<commit_message>
adult TOD norms through pan
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/lem_sum-adult-raw-ss-lookup-tabbed-age.xlsx
+++ b/OUTPUT-FILES/NORMS/TODC_adult_10.28.21_for norms/lem_sum-adult-raw-ss-lookup-tabbed-age.xlsx
@@ -356,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,127 +376,127 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>43</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>126</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -504,7 +504,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -520,7 +520,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -528,9 +528,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -541,7 +549,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -561,127 +569,127 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -689,7 +697,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -697,7 +705,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -705,7 +713,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -713,9 +721,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -726,7 +742,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -746,15 +762,15 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>56</v>
@@ -762,111 +778,111 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -874,7 +890,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -882,7 +898,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -890,7 +906,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -898,9 +914,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -911,7 +935,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -931,127 +955,127 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>81</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1059,7 +1083,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1067,7 +1091,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1075,7 +1099,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1083,9 +1107,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -1096,7 +1128,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1116,127 +1148,127 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>91</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>123</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>129</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1244,7 +1276,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1252,7 +1284,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1260,7 +1292,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1268,9 +1300,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>
@@ -1281,7 +1321,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1301,127 +1341,127 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <v>72</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>79</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>92</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>97</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>103</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>108</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>113</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <v>130</v>
@@ -1429,7 +1469,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <v>130</v>
@@ -1437,7 +1477,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
         <v>130</v>
@@ -1445,7 +1485,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>130</v>
@@ -1453,9 +1493,17 @@
     </row>
     <row r="21">
       <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>130</v>
       </c>
     </row>

</xml_diff>